<commit_message>
minor changes for axis control PCB
</commit_message>
<xml_diff>
--- a/Electronics/Main_board/BOM/BOM.xlsx
+++ b/Electronics/Main_board/BOM/BOM.xlsx
@@ -79,7 +79,7 @@
     <t xml:space="preserve">LED Strip</t>
   </si>
   <si>
-    <t xml:space="preserve">Power MOSFET control for LED</t>
+    <t xml:space="preserve">Power MOSFET control board</t>
   </si>
   <si>
     <t xml:space="preserve">TOTAL</t>
@@ -404,10 +404,10 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="114" zoomScaleNormal="114" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13:K13"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.86"/>

</xml_diff>